<commit_message>
Added Controls page to options so you can see controls (in level only so far) Added a new sprite sheet for player (included up and down idle/att.
</commit_message>
<xml_diff>
--- a/Assets/Database/Excel/Items.xlsx
+++ b/Assets/Database/Excel/Items.xlsx
@@ -404,7 +404,7 @@
     <t>The strongest of all the Magic Keys in existence. With this you may be able to defeat any foe.</t>
   </si>
   <si>
-    <t>Sandels</t>
+    <t>Leather Hat</t>
   </si>
   <si>
     <t>Armor</t>
@@ -413,7 +413,7 @@
     <t>Shoes</t>
   </si>
   <si>
-    <t>A pair of shoes, made out of leather. Said not to be too protective.</t>
+    <t>A hat made out of leather. Said not to be too protective.</t>
   </si>
   <si>
     <t>Leather Gloves</t>
@@ -434,10 +434,10 @@
     <t>A strap made out of leather. Said not to be too protective.</t>
   </si>
   <si>
-    <t>Bronze Shoes</t>
-  </si>
-  <si>
-    <t>A pair of shoes made out of bronze. Said to be protective, but not too durable.</t>
+    <t>Baseball Cap</t>
+  </si>
+  <si>
+    <t>A hat said to help you “Defeat them all”.</t>
   </si>
   <si>
     <t>Bronze Gloves</t>
@@ -452,10 +452,10 @@
     <t>A strap made out of bronze. Said to be protective, but not too durable.</t>
   </si>
   <si>
-    <t>Iron Shoes</t>
-  </si>
-  <si>
-    <t>A pair of shoes made out of iron. Protective &amp; Durable.</t>
+    <t>Bandana</t>
+  </si>
+  <si>
+    <t>A tied up bandana. You’re getting serious now, don’t forget about stealth mode.</t>
   </si>
   <si>
     <t>Iron Gloves</t>
@@ -470,10 +470,10 @@
     <t>A strap made out of iron. Protective &amp; Durable.</t>
   </si>
   <si>
-    <t>Steel Shoes</t>
-  </si>
-  <si>
-    <t>A pair of shoes made ouf of steel. The most protective of all the metal equipments.</t>
+    <t>Elf Cap</t>
+  </si>
+  <si>
+    <t>With this hat you should be able to help the princess and get your Master Daggers.</t>
   </si>
   <si>
     <t>Steel Gloves</t>
@@ -488,10 +488,10 @@
     <t>A strap made out of steel. The most protective of all the metal equipments.</t>
   </si>
   <si>
-    <t>Blood Shoes</t>
-  </si>
-  <si>
-    <t>A pair of shoes, infused with the blood of an unknown source. Rumored to increase your strength.</t>
+    <t>Plumber Hat</t>
+  </si>
+  <si>
+    <t>You better save the princess again, I can’t understand why she won’t stop getting captured either.</t>
   </si>
   <si>
     <t>Blood Gloves</t>
@@ -506,13 +506,13 @@
     <t>A strap, infused with the blood of an unknown source. Rumored to increase your strength.</t>
   </si>
   <si>
-    <t>Love Shoes</t>
+    <t>Kingdom Crown</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>A pair of shoes, infused with love from an unknown source. Rumored to increase your intelligence.</t>
+    <t>With the Kingdom crown and magic keys you should be able to fully unlock your Hearts potential.</t>
   </si>
   <si>
     <t>Love Gloves</t>
@@ -857,7 +857,7 @@
     <xf numFmtId="1" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -884,7 +884,7 @@
     <xf numFmtId="1" fontId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>

</xml_diff>